<commit_message>
All changes through Jul 2024
</commit_message>
<xml_diff>
--- a/STEP3IncomingData.xlsx
+++ b/STEP3IncomingData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="126">
   <si>
     <t>id</t>
   </si>
@@ -97,205 +97,301 @@
     <t>6401Basswood</t>
   </si>
   <si>
-    <t>WF Bus Credit AUTO PAY 240620 90469914333885 GUPTA,NEERAJ</t>
-  </si>
-  <si>
-    <t>OnePlus Realty G SIGONFILE 061424 YFDXJ2 Midway Inn LLC</t>
-  </si>
-  <si>
-    <t>ONLINE TRANSFER TO GUPTA N REF #IB0NJHQSPH EVERYDAY CHECKING MIDWAY REFRGTR PURCHASE LOWES CRD KODIAK</t>
-  </si>
-  <si>
-    <t>RECURRING PAYMENT AUTHORIZED ON 06/12 Spectrum 855-707-7328 MO S584164550672936 CARD 4162</t>
-  </si>
-  <si>
-    <t>BUSINESS TO BUSINESS ACH CITY OFARLINGTON UTILITYIVR 240610 6060306 MIDWAY INN *LLC</t>
-  </si>
-  <si>
-    <t>ONLINE TRANSFER TO GUPTA N REF #IB0NHL3HPN EVERYDAY CHECKING MIDWAY EXPENSES MAY THRU ONEPLUS PM</t>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2VK6BX TRULO MONTHLY PM FEE MIDWAY INN</t>
+  </si>
+  <si>
+    <t>RECURRING PAYMENT AUTHORIZED ON 07/29 DNH*GODADDY#321752 480-5058855 AZ S304211626202408 CARD 4162</t>
+  </si>
+  <si>
+    <t>Instant Pmt from ONEPLUS REALTY GROUP LLC on 07/30 Ref#20240730021000021P1BRJPC00520076928</t>
+  </si>
+  <si>
+    <t>CHECK # 1011</t>
+  </si>
+  <si>
+    <t>WF Bus Credit AUTO PAY 240721 90469914333885 GUPTA,NEERAJ</t>
+  </si>
+  <si>
+    <t>Instant Pmt from ONEPLUS REALTY GROUP LLC on 07/21 Ref#20240721021000021P1BRJPC00510064841</t>
+  </si>
+  <si>
+    <t>RECURRING PAYMENT AUTHORIZED ON 07/14 DNH*GODADDY#318938 480-5058855 AZ S584196656484877 CARD 4162</t>
+  </si>
+  <si>
+    <t>RECURRING PAYMENT AUTHORIZED ON 07/12 Spectrum 855-707-7328 MO S584194554099969 CARD 4162</t>
+  </si>
+  <si>
+    <t>BUSINESS TO BUSINESS ACH CITY OFARLINGTON UTILITYIVR 240710 5743289 MIDWAY INN *LLC</t>
   </si>
   <si>
     <t>BUSINESS TO BUSINESS ACH Lument7313 ACH 490011466</t>
   </si>
   <si>
-    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NDPY8PQ TRULO MONTHLY PM FEE MIDWAY INN</t>
-  </si>
-  <si>
-    <t>OnePlus Realty G SIGONFILE 061124 91HNJ2 Meadow View Homes LLC</t>
-  </si>
-  <si>
-    <t>SERVICEMAC PMT MTGE PAYMT 060124 5114002632 PARUL GUPTA</t>
-  </si>
-  <si>
-    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NDQFJ9V 108MV TO TRULO PROPERTY MANAGEMENT</t>
-  </si>
-  <si>
-    <t>OnePlus Realty G SIGONFILE 061124 B1HNJ2 Meadow View Homes LLC</t>
-  </si>
-  <si>
-    <t>RECURRING TRANSFER TO MEADOW VIEW HOMES LLC REF #OP0NHDZ6KM BUSINESS MARKET RATE SAVINGS 116 MV CHK TO SAV</t>
-  </si>
-  <si>
-    <t>NEWREZ-SHELLPOIN ACH PMT 240531 0683624456 GUPTA PARUL</t>
-  </si>
-  <si>
-    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NDQHBFB 116MV TO TRULO PROPERTY MANAGEMENT</t>
+    <t>PURCHASE AUTHORIZED ON 07/06 Mobimatter Abu Dhabi ARE S464188635540782 CARD 4162</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ5FSZ3 TRULO MONTHLY PM FEE MIDWAY INN</t>
+  </si>
+  <si>
+    <t>SERVICEMAC PMT MTGE PAYMT 080124 5114002632 PARUL GUPTA</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2VCNRL 108MV TO TRULO PROPERTY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>SERVICEMAC PMT MTGE PAYMT 070124 5114002632 PARUL GUPTA</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ58NCB 108MV TO TRULO PROPERTY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>NEWREZ-SHELLPOIN ACH PMT 240731 0683624456 GUPTA PARUL</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2V3PQ8 116MV TO TRULO PROPERTY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>OnePlus Realty G SIGONFILE 071024 4TRBL2 Meadow View Homes LLC</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO MEADOW VIEW HOMES LLC REF #OP0NSR3SBH BUSINESS MARKET RATE SAVINGS 116 MV CHK TO SAV</t>
+  </si>
+  <si>
+    <t>NEWREZ-SHELLPOIN ACH PMT 240630 0683624456 GUPTA PARUL</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ6F5RZ 116MV TO TRULO PROPERTY MANAGEMENT</t>
   </si>
   <si>
     <t>INTEREST PAYMENT</t>
   </si>
   <si>
-    <t>OnePlus Realty G SIGONFILE 061124 C1HNJ2 Pagoda Homes (Newton)</t>
-  </si>
-  <si>
-    <t>NEWREZ-SHELLPOIN ACH PMT 240531 0683856942 GUPTA PARUL</t>
-  </si>
-  <si>
-    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NDQJP56 NEWTON TO TRULO PROPERTY MANAGEMENT</t>
-  </si>
-  <si>
-    <t>FOREMOST EPM PYMT 240616 3810091873545 VIVEK JADHAV</t>
-  </si>
-  <si>
-    <t>OnePlus Realty G SIGONFILE 061124 F1HNJ2 Pagoda Homes LLC (Rose</t>
-  </si>
-  <si>
-    <t>PENNYMAC CASH Jun 24 8028350915-0054 1316 Rosemon</t>
-  </si>
-  <si>
-    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NDPX8HZ ROSEMON TO TRULO PROPERTY MANAGEMENT</t>
-  </si>
-  <si>
-    <t>OnePlus Realty G SIGONFILE 061124 81HNJ2 Meadow View Homes LLC</t>
-  </si>
-  <si>
-    <t>PENNYMAC CASH Jun 24 8028352704-0054 104 Meadow</t>
-  </si>
-  <si>
-    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NDQ85ZP 104MV TO TRULO PROPERTY MANAGEMENT</t>
-  </si>
-  <si>
-    <t>RECURRING TRANSFER FROM MEADOW VIEW HOMES LLC REF #OP0NHDZ6KM BUSINESS CHECKING 116 MV CHK TO SAV</t>
-  </si>
-  <si>
-    <t>ONLINE TRANSFER FROM GUPTA P REF #IB0NG473XQ PLATINUM SAVINGS FUNDING PARKS</t>
-  </si>
-  <si>
-    <t>OVERDRAFT FEE FOR A TRANSACTION POSTED ON 06/03 $733.95 SERVICEMAC PMT MTGE PAYMT 060124 5114002634 PARUL GUPTA</t>
-  </si>
-  <si>
-    <t>SERVICEMAC PMT MTGE PAYMT 060124 5114002634 PARUL GUPTA</t>
-  </si>
-  <si>
-    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NDQ6CMD PARKS TO TRULO PROPERTY MANAGEMENT</t>
-  </si>
-  <si>
-    <t>OnePlus Realty G SIGONFILE 061124 D1HNJ2 Pagoda Homes LLC (108</t>
-  </si>
-  <si>
-    <t>FREEDOM MTG PYMTS 060324 0129201927 NEERAJ GUPTA</t>
-  </si>
-  <si>
-    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NDQKR6D TRULO PROPERTY MANAGEMENT MONTHLY FEE</t>
-  </si>
-  <si>
-    <t>OnePlus Realty G SIGONFILE 061124 61HNJ2 Meadow View Homes LLC</t>
-  </si>
-  <si>
-    <t>JPMORGAN CHASE CHASE ACH 060124 4027425045 MEADOW VIEW HOMES LLC</t>
-  </si>
-  <si>
-    <t>WT FED#06040 BANK 7 /FTR/BNF=Eddy Estates LLC SRF# OW00004593387892 TRN#240613133471 RFB# OW00004593387892</t>
-  </si>
-  <si>
-    <t>WIRE TRANS SVC CHARGE - SEQUENCE: 240613133471 SRF# OW00004593387892 TRN#240613133471 RFB# OW00004593387892</t>
-  </si>
-  <si>
-    <t>ONLINE TRANSFER TO PAGODA HOMES LLC REF #IB0NG473XQ BUSINESS CHECKING FUNDING PARKS</t>
-  </si>
-  <si>
-    <t>SERVICEMAC PMT MTGE PAYMT 060124 5114002633 PARUL GUPTA</t>
-  </si>
-  <si>
-    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NDQ3VW7 BREWER TO TRULO PROPERTY MANAGEMENT</t>
-  </si>
-  <si>
-    <t>OnePlus Realty G SIGONFILE 061124 J1HNJ2 Pagoda Homes (Wintergr</t>
-  </si>
-  <si>
-    <t>PENNYMAC CASH Jun 24 8028351602-0053 vivek jadhav</t>
-  </si>
-  <si>
-    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NDQ8K3K WINTERGREEN TO TRULO PROPERTY MANAGEMENT</t>
-  </si>
-  <si>
-    <t>Online Transfer from CHK ...6571 transaction#: 20967326607</t>
-  </si>
-  <si>
-    <t>Online Transfer to CHK ...5031 transaction#: 20967326607 06/03</t>
-  </si>
-  <si>
-    <t>Online Payment 20926681363 To CHASE HOME MORTGAGE 06/28</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240611 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000015125058 EED:240612   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1645125058TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240610 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000018389590 EED:240611   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1638389590TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240610 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000018389587 EED:240611   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1638389587TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240610 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000018389591 EED:240611   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1638389591TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:061124 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926088253631 EED:240611   IND ID:71HNJ2                       IND NAME:Pagoda Homes LLC (Jame                                                                                       469-867-9837 TRN: 1638253631TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240603 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000016950664 EED:240604   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1566950664TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240603 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000016950750 EED:240604   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1566950750TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240603 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000016896172 EED:240604   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1566896172TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240603 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000016896194 EED:240604   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1566896194TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:JPMORGAN CHASE         ORIG ID:1000008113 DESC DATE:060124 CO ENTRY DESCR:CHASE ACH SEC:PPD    TRACE#:021000026773208 EED:240603   IND ID:                             IND NAME:MEADOW VIEW HOMES LLC TRN: 1556773208TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:061124 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926088253633 EED:240611   IND ID:H1HNJ2                       IND NAME:Meadow View Homes LLC                                                                                        469-867-9837 TRN: 1638253633TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:PENNYMAC               ORIG ID:1262049351 DESC DATE:Jun 24 CO ENTRY DESCR:CASH      SEC:WEB    TRACE#:021000023691162 EED:240603   IND ID:8028351082-0054              IND NAME:8604 Wagon TRN: 1553691162TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:061124 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926088253632 EED:240611   IND ID:G1HNJ2                       IND NAME:Meadow View Homes LLC                                                                                        469-867-9837 TRN: 1638253632TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:SERVICEMAC PMT         ORIG ID:4823070213 DESC DATE:060124 CO ENTRY DESCR:MTGE PAYMTSEC:PPD    TRACE#:091000014238430 EED:240603   IND ID:                             IND NAME:PARUL GUPTA TRN: 1554238430TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240611 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000015125053 EED:240612   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1645125053TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240610 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000018389588 EED:240611   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1638389588TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:061124 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926088253630 EED:240611   IND ID:51HNJ2                       IND NAME:Pagoda Homes LLC (Bass                                                                                       469-867-9837 TRN: 1638253630TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:TARA ENERGY            ORIG ID:0000267208 DESC DATE:240607 CO ENTRY DESCR:UTILITIES SEC:WEB    TRACE#:021000021237423 EED:240607   IND ID:5010272                      IND NAME:NEERAJ *GUPTA                                                                                                866-438-8272 TRN: 1591237423TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:TARA ENERGY            ORIG ID:0000267208 DESC DATE:240604 CO ENTRY DESCR:UTILITIES SEC:WEB    TRACE#:021000021882489 EED:240604   IND ID:3925259                      IND NAME:NEERAJ *GUPTA                                                                                                866-438-8272 TRN: 1561882489TC</t>
-  </si>
-  <si>
-    <t>ORIG CO NAME:NEWREZ-SHELLPOIN       ORIG ID:6371542226 DESC DATE:240531 CO ENTRY DESCR:ACH PMT   SEC:PPD    TRACE#:028000089777557 EED:240603   IND ID:                             IND NAME:JADHAV VIVEK TRN: 1559777557TC</t>
+    <t>NEWREZ-SHELLPOIN ACH PMT 240731 0683856942 GUPTA PARUL</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2VKXGK NEWTON TO TRULO PROPERTY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>OnePlus Realty G SIGONFILE 073124 RZKLM2 Pagoda Homes (Newton)</t>
+  </si>
+  <si>
+    <t>OnePlus Realty G SIGONFILE 071024 5TRBL2 Pagoda Homes (Newton)</t>
+  </si>
+  <si>
+    <t>NEWREZ-SHELLPOIN ACH PMT 240630 0683856942 GUPTA PARUL</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ6T9P2 NEWTON TO TRULO PROPERTY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>PENNYMAC CASH Aug 24 8028350915-0056 1316 Rosemon</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2TXGGY ROSEMON TO TRULO PROPERTY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>FOREMOST EPM PYMT 240726 3810091873545 VIVEK JADHAV</t>
+  </si>
+  <si>
+    <t>OnePlus Realty G SIGONFILE 071024 7TRBL2 Pagoda Homes LLC (Rose</t>
+  </si>
+  <si>
+    <t>PENNYMAC CASH Jul 24 8028350915-0055 1316 Rosemon</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ54Y3C ROSEMON TO TRULO PROPERTY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>PENNYMAC CASH Aug 24 8028352704-0056 104 Meadow</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2VMZ9B 104MV TO TRULO PROPERTY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>OnePlus Realty G SIGONFILE 071024 3TRBL2 Meadow View Homes LLC</t>
+  </si>
+  <si>
+    <t>PENNYMAC CASH Jul 24 8028352704-0055 104 Meadow</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ55Y6Q 104MV TO TRULO PROPERTY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER FROM MEADOW VIEW HOMES LLC REF #OP0NSR3SBH BUSINESS CHECKING 116 MV CHK TO SAV</t>
+  </si>
+  <si>
+    <t>SERVICEMAC PMT MTGE PAYMT 080124 5114002634 PARUL GUPTA</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2TT3W6 PARKS TO TRULO PROPERTY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>SERVICEMAC PMT MTGE PAYMT 070124 5114002634 PARUL GUPTA</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ5P3GX PARKS TO TRULO PROPERTY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>FREEDOM MTG PYMTS 080124 0129201927 NEERAJ GUPTA</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2VHFSF TRULO PROPERTY MANAGEMENT MONTHLY FEE</t>
+  </si>
+  <si>
+    <t>OnePlus Realty G SIGONFILE 071024 6TRBL2 Pagoda Homes LLC (108</t>
+  </si>
+  <si>
+    <t>FREEDOM MTG PYMTS 070124 0129201927 NEERAJ GUPTA</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ59FR9 TRULO PROPERTY MANAGEMENT MONTHLY FEE</t>
+  </si>
+  <si>
+    <t>JPMORGAN CHASE CHASE ACH 080124 4027425045 MEADOW VIEW HOMES LLC</t>
+  </si>
+  <si>
+    <t>OnePlus Realty G SIGONFILE 071024 1TRBL2 Meadow View Homes LLC</t>
+  </si>
+  <si>
+    <t>JPMORGAN CHASE CHASE ACH 070124 4027425045 MEADOW VIEW HOMES LLC</t>
+  </si>
+  <si>
+    <t>ZELLE TO PROPERTY MANAGEMENT TRULO ON 07/12 REF #RP0SF2YHM4 ATTORNEY FEE WIRE THRU CHASE FOR CHAKRI</t>
+  </si>
+  <si>
+    <t>ONLINE TRANSFER TO GUPTA N REF #IB0NTSRLJC EVERYDAY CHECKING CHAKRI WIRE XFER FEE</t>
+  </si>
+  <si>
+    <t>ONLINE TRANSFER FROM GUPTA N REF #IB0NTSQSGR EVERYDAY CHECKING CHAKRI PAID ATTORNEY FEE</t>
+  </si>
+  <si>
+    <t>ONLINE TRANSFER FROM GUPTA N REF #IB0NTSQG3V EVERYDAY CHECKING CHAKRI INT JULY</t>
+  </si>
+  <si>
+    <t>ONLINE TRANSFER TO GUPTA N REF #IB0NT79WFZ EVERYDAY CHECKING CHAKRI AND SRAVYA</t>
+  </si>
+  <si>
+    <t>ONLINE TRANSFER TO GUPTA N REF #IB0NT74JWP EVERYDAY CHECKING CHAKRADER AND SRAVYA</t>
+  </si>
+  <si>
+    <t>SERVICEMAC PMT MTGE PAYMT 080124 5114002633 PARUL GUPTA</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2TWZK5 BREWER TO TRULO PROPERTY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>OnePlus Realty G SIGONFILE 073124 PZKLM2 Neeraj Gupta (Brewer)</t>
+  </si>
+  <si>
+    <t>OnePlus Realty G SIGONFILE 071024 0TRBL2 Neeraj Gupta (Brewer)</t>
+  </si>
+  <si>
+    <t>SERVICEMAC PMT MTGE PAYMT 070124 5114002633 PARUL GUPTA</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ59Q3N BREWER TO TRULO PROPERTY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>PENNYMAC CASH Aug 24 8028351602-0055 vivek jadhav</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2V8M6F WINTERGREEN TO TRULO PROPERTY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>OnePlus Realty G SIGONFILE 071024 BTRBL2 Pagoda Homes (Wintergr</t>
+  </si>
+  <si>
+    <t>PENNYMAC CASH Jul 24 8028351602-0054 vivek jadhav</t>
+  </si>
+  <si>
+    <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ68C2D WINTERGREEN TO TRULO PROPERTY MANAGEMENT</t>
+  </si>
+  <si>
+    <t>Online Transfer from CHK ...6571 transaction#: 21572783954</t>
+  </si>
+  <si>
+    <t>Zelle payment from TRULO PROPERTY MANAGEMENT LLC 21572866504</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:CHASE CREDIT CRD       ORIG ID:4760039224 DESC DATE:240728 CO ENTRY DESCR:AUTOPAYBUSSEC:PPD    TRACE#:021000024987396 EED:240729   IND ID:                             IND NAME:GUPTA NEERAJ TRN: 2114987396TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:CHASE CREDIT CRD       ORIG ID:4760039224 DESC DATE:240628 CO ENTRY DESCR:AUTOPAYBUSSEC:PPD    TRACE#:021000020238031 EED:240701   IND ID:                             IND NAME:GUPTA NEERAJ TRN: 1830238031TC</t>
+  </si>
+  <si>
+    <t>Online Transfer to CHK ...5031 transaction#: 21572783954 07/31</t>
+  </si>
+  <si>
+    <t>Online Payment 21229559529 To CHASE HOME MORTGAGE 07/31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHECK 2032  </t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:VRBO                   ORIG ID:9872667522 DESC DATE:240719 CO ENTRY DESCR:PAYMENT   SEC:PPD    TRACE#:031101111714572 EED:240722   IND ID:                             IND NAME:Neeraj Gupta TRN: 2041714572TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240709 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000018411692 EED:240710   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1928411692TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240709 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000018411685 EED:240710   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1928411685TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240709 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000018411691 EED:240710   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1928411691TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240709 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000018411687 EED:240710   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1928411687TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:071024 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926088315743 EED:240710   IND ID:2TRBL2                       IND NAME:Pagoda Homes LLC (Jame                                                                                       469-867-9837 TRN: 1928315743TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240702 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000010929691 EED:240703   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1850929691TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240702 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000010926310 EED:240703   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1850926310TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240702 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000010926327 EED:240703   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1850926327TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240702 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000010929696 EED:240703   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1850929696TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:JPMORGAN CHASE         ORIG ID:1000008113 DESC DATE:080124 CO ENTRY DESCR:CHASE ACH SEC:PPD    TRACE#:021000029832472 EED:240801   IND ID:                             IND NAME:MEADOW VIEW HOMES LLC TRN: 2149832472TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:073124 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926084765326 EED:240731   IND ID:QZKLM2                       IND NAME:Meadow View Homes LLC                                                                                        469-867-9837 TRN: 2134765326TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:JPMORGAN CHASE         ORIG ID:1000008113 DESC DATE:070124 CO ENTRY DESCR:CHASE ACH SEC:PPD    TRACE#:021000020928596 EED:240701   IND ID:                             IND NAME:MEADOW VIEW HOMES LLC TRN: 1830928596TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:PENNYMAC               ORIG ID:1262049351 DESC DATE:Aug 24 CO ENTRY DESCR:CASH      SEC:WEB    TRACE#:021000021437718 EED:240801   IND ID:8028351082-0056              IND NAME:8604 Wagon TRN: 2141437718TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:071024 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926088315745 EED:240710   IND ID:9TRBL2                       IND NAME:Meadow View Homes LLC                                                                                        469-867-9837 TRN: 1928315745TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:PENNYMAC               ORIG ID:1262049351 DESC DATE:Jul 24 CO ENTRY DESCR:CASH      SEC:WEB    TRACE#:021000020542007 EED:240701   IND ID:8028351082-0055              IND NAME:8604 Wagon TRN: 1830542007TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:SERVICEMAC PMT         ORIG ID:4823070213 DESC DATE:080124 CO ENTRY DESCR:MTGE PAYMTSEC:PPD    TRACE#:091000019427854 EED:240801   IND ID:                             IND NAME:PARUL GUPTA TRN: 2149427854TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:071024 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926088315744 EED:240710   IND ID:8TRBL2                       IND NAME:Meadow View Homes LLC                                                                                        469-867-9837 TRN: 1928315744TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:SERVICEMAC PMT         ORIG ID:4823070213 DESC DATE:070124 CO ENTRY DESCR:MTGE PAYMTSEC:PPD    TRACE#:091000010669125 EED:240701   IND ID:                             IND NAME:PARUL GUPTA TRN: 1830669125TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:NEWREZ-SHELLPOIN       ORIG ID:6371542226 DESC DATE:240731 CO ENTRY DESCR:ACH PMT   SEC:PPD    TRACE#:028000083659872 EED:240801   IND ID:                             IND NAME:JADHAV VIVEK TRN: 2143659872TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:071024 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926088315742 EED:240710   IND ID:ZSRBL2                       IND NAME:Pagoda Homes LLC (Bass                                                                                       469-867-9837 TRN: 1928315742TC</t>
+  </si>
+  <si>
+    <t>ORIG CO NAME:NEWREZ-SHELLPOIN       ORIG ID:6371542226 DESC DATE:240630 CO ENTRY DESCR:ACH PMT   SEC:PPD    TRACE#:028000083248476 EED:240701   IND ID:                             IND NAME:JADHAV VIVEK TRN: 1833248476TC</t>
   </si>
 </sst>
 </file>
@@ -657,7 +753,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -688,13 +784,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>45463</v>
+        <v>45505</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
       </c>
       <c r="E2">
-        <v>-804.95</v>
+        <v>-1500</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -705,13 +801,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="2">
-        <v>45457</v>
+        <v>45503</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
       </c>
       <c r="E3">
-        <v>28291.43</v>
+        <v>-204.42</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -722,13 +818,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="2">
-        <v>45456</v>
+        <v>45503</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
       </c>
       <c r="E4">
-        <v>-246</v>
+        <v>17028.44</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -739,13 +835,13 @@
         <v>5</v>
       </c>
       <c r="C5" s="2">
-        <v>45456</v>
+        <v>45496</v>
       </c>
       <c r="D5" t="s">
         <v>30</v>
       </c>
       <c r="E5">
-        <v>-77.28</v>
+        <v>-800</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -756,13 +852,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="2">
-        <v>45454</v>
+        <v>45495</v>
       </c>
       <c r="D6" t="s">
         <v>31</v>
       </c>
       <c r="E6">
-        <v>-760.8</v>
+        <v>-136.07</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -773,13 +869,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="2">
-        <v>45453</v>
+        <v>45495</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
       </c>
       <c r="E7">
-        <v>-4001</v>
+        <v>800</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -790,13 +886,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="2">
-        <v>45449</v>
+        <v>45488</v>
       </c>
       <c r="D8" t="s">
         <v>33</v>
       </c>
       <c r="E8">
-        <v>-9368.889999999999</v>
+        <v>-22.17</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -807,690 +903,690 @@
         <v>5</v>
       </c>
       <c r="C9" s="2">
-        <v>45446</v>
+        <v>45488</v>
       </c>
       <c r="D9" t="s">
         <v>34</v>
       </c>
       <c r="E9">
-        <v>-1500</v>
+        <v>-77.28</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2">
-        <v>45454</v>
+        <v>45484</v>
       </c>
       <c r="D10" t="s">
         <v>35</v>
       </c>
       <c r="E10">
-        <v>1850</v>
+        <v>-956.2</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="2">
-        <v>45446</v>
+        <v>45481</v>
       </c>
       <c r="D11" t="s">
         <v>36</v>
       </c>
       <c r="E11">
-        <v>-748.9299999999999</v>
+        <v>-9212.299999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="2">
-        <v>45446</v>
+        <v>45481</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
       </c>
       <c r="E12">
-        <v>-75</v>
+        <v>-11.63</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2">
-        <v>45454</v>
+        <v>45474</v>
       </c>
       <c r="D13" t="s">
         <v>38</v>
       </c>
       <c r="E13">
-        <v>99</v>
+        <v>-1500</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="2">
-        <v>45453</v>
+        <v>45505</v>
       </c>
       <c r="D14" t="s">
         <v>39</v>
       </c>
       <c r="E14">
-        <v>-150</v>
+        <v>-748.9299999999999</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="D15" t="s">
         <v>40</v>
       </c>
       <c r="E15">
-        <v>-456.02</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="2">
-        <v>45446</v>
+        <v>45474</v>
       </c>
       <c r="D16" t="s">
         <v>41</v>
       </c>
       <c r="E16">
-        <v>-75</v>
+        <v>-748.9299999999999</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C17" s="2">
-        <v>45471</v>
+        <v>45474</v>
       </c>
       <c r="D17" t="s">
         <v>42</v>
       </c>
       <c r="E17">
-        <v>0.02</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C18" s="2">
-        <v>45454</v>
+        <v>45505</v>
       </c>
       <c r="D18" t="s">
         <v>43</v>
       </c>
       <c r="E18">
-        <v>1593.5</v>
+        <v>-456.02</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C19" s="2">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="D19" t="s">
         <v>44</v>
       </c>
       <c r="E19">
-        <v>-563.38</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C20" s="2">
-        <v>45446</v>
+        <v>45483</v>
       </c>
       <c r="D20" t="s">
         <v>45</v>
       </c>
       <c r="E20">
-        <v>-75</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C21" s="2">
-        <v>45460</v>
+        <v>45482</v>
       </c>
       <c r="D21" t="s">
         <v>46</v>
       </c>
       <c r="E21">
-        <v>-356.49</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C22" s="2">
-        <v>45454</v>
+        <v>45474</v>
       </c>
       <c r="D22" t="s">
         <v>47</v>
       </c>
       <c r="E22">
-        <v>3878</v>
+        <v>-456.02</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C23" s="2">
-        <v>45446</v>
+        <v>45474</v>
       </c>
       <c r="D23" t="s">
         <v>48</v>
       </c>
       <c r="E23">
-        <v>-963.16</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C24" s="2">
-        <v>45446</v>
+        <v>45504</v>
       </c>
       <c r="D24" t="s">
         <v>49</v>
       </c>
       <c r="E24">
-        <v>-150</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C25" s="2">
-        <v>45454</v>
+        <v>45505</v>
       </c>
       <c r="D25" t="s">
         <v>50</v>
       </c>
       <c r="E25">
-        <v>1700</v>
+        <v>-563.38</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C26" s="2">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="D26" t="s">
         <v>51</v>
       </c>
       <c r="E26">
-        <v>-730.2</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C27" s="2">
-        <v>45446</v>
+        <v>45504</v>
       </c>
       <c r="D27" t="s">
         <v>52</v>
       </c>
       <c r="E27">
-        <v>-75</v>
+        <v>1748.17</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C28" s="2">
-        <v>45471</v>
+        <v>45483</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E28">
-        <v>0.02</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C29" s="2">
-        <v>45453</v>
+        <v>45474</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E29">
-        <v>150</v>
+        <v>-563.38</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C30" s="2">
-        <v>45448</v>
+        <v>45474</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E30">
-        <v>2500</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C31" s="2">
-        <v>45447</v>
+        <v>45506</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E31">
-        <v>-35</v>
+        <v>-963.16</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C32" s="2">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="D32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E32">
-        <v>-733.95</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C33" s="2">
-        <v>45446</v>
+        <v>45502</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E33">
-        <v>-75</v>
+        <v>-414</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C34" s="2">
-        <v>45454</v>
+        <v>45483</v>
       </c>
       <c r="D34" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E34">
-        <v>1525</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C35" s="2">
-        <v>45446</v>
+        <v>45475</v>
       </c>
       <c r="D35" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E35">
-        <v>-726.97</v>
+        <v>-963.16</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C36" s="2">
-        <v>45446</v>
+        <v>45474</v>
       </c>
       <c r="D36" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E36">
-        <v>-75</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C37" s="2">
-        <v>45471</v>
+        <v>45506</v>
       </c>
       <c r="D37" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="E37">
-        <v>0.06</v>
+        <v>-730.2</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C38" s="2">
-        <v>45454</v>
+        <v>45505</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E38">
-        <v>2500</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C39" s="2">
-        <v>45446</v>
+        <v>45483</v>
       </c>
       <c r="D39" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E39">
-        <v>-947.72</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C40" s="2">
-        <v>45471</v>
+        <v>45475</v>
       </c>
       <c r="D40" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="E40">
-        <v>0.24</v>
+        <v>-730.2</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C41" s="2">
-        <v>45471</v>
+        <v>45474</v>
       </c>
       <c r="D41" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E41">
-        <v>31.42</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C42" s="2">
-        <v>45456</v>
+        <v>45504</v>
       </c>
       <c r="D42" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E42">
-        <v>-98000</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43">
-        <v>129</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C43" s="2">
-        <v>45456</v>
+        <v>45482</v>
       </c>
       <c r="D43" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E43">
-        <v>-25</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C44" s="2">
-        <v>45448</v>
+        <v>45505</v>
       </c>
       <c r="D44" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E44">
-        <v>-2500</v>
+        <v>-733.95</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C45" s="2">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="D45" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E45">
-        <v>-711.48</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C46" s="2">
-        <v>45446</v>
+        <v>45474</v>
       </c>
       <c r="D46" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E46">
-        <v>-75</v>
+        <v>-733.95</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C47" s="2">
-        <v>45454</v>
+        <v>45474</v>
       </c>
       <c r="D47" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E47">
-        <v>1545.21</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48">
-        <v>148</v>
+        <v>100</v>
       </c>
       <c r="B48" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C48" s="2">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="D48" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E48">
-        <v>-694.01</v>
+        <v>-726.97</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C49" s="2">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="D49" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E49">
         <v>-75</v>
@@ -1498,392 +1594,936 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50">
-        <v>154</v>
+        <v>102</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C50" s="2">
-        <v>45446</v>
+        <v>45483</v>
       </c>
       <c r="D50" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E50">
-        <v>500</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51">
-        <v>204</v>
+        <v>103</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C51" s="2">
-        <v>45446</v>
+        <v>45474</v>
       </c>
       <c r="D51" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E51">
-        <v>-500</v>
+        <v>-726.97</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52">
-        <v>282</v>
+        <v>104</v>
       </c>
       <c r="B52" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C52" s="2">
-        <v>45471</v>
+        <v>45474</v>
       </c>
       <c r="D52" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E52">
-        <v>-1118.25</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53">
-        <v>283</v>
+        <v>109</v>
       </c>
       <c r="B53" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C53" s="2">
-        <v>45455</v>
+        <v>45505</v>
       </c>
       <c r="D53" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E53">
-        <v>-128.12</v>
+        <v>-947.72</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54">
-        <v>284</v>
+        <v>110</v>
       </c>
       <c r="B54" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C54" s="2">
-        <v>45454</v>
+        <v>45504</v>
       </c>
       <c r="D54" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="E54">
-        <v>-55.45</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55">
-        <v>285</v>
+        <v>111</v>
       </c>
       <c r="B55" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C55" s="2">
-        <v>45454</v>
+        <v>45483</v>
       </c>
       <c r="D55" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E55">
-        <v>-55.91</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56">
-        <v>286</v>
+        <v>112</v>
       </c>
       <c r="B56" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C56" s="2">
-        <v>45454</v>
+        <v>45474</v>
       </c>
       <c r="D56" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E56">
-        <v>-69.43000000000001</v>
+        <v>-947.72</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57">
-        <v>287</v>
+        <v>118</v>
       </c>
       <c r="B57" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C57" s="2">
-        <v>45454</v>
+        <v>45504</v>
       </c>
       <c r="D57" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="E57">
-        <v>1190.06</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58">
-        <v>288</v>
+        <v>121</v>
       </c>
       <c r="B58" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C58" s="2">
-        <v>45447</v>
+        <v>45504</v>
       </c>
       <c r="D58" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="E58">
-        <v>-74.95</v>
+        <v>158.77</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59">
-        <v>289</v>
+        <v>122</v>
       </c>
       <c r="B59" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C59" s="2">
-        <v>45447</v>
+        <v>45485</v>
       </c>
       <c r="D59" t="s">
         <v>80</v>
       </c>
       <c r="E59">
-        <v>-76.48999999999999</v>
+        <v>-450</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60">
-        <v>290</v>
+        <v>123</v>
       </c>
       <c r="B60" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C60" s="2">
-        <v>45447</v>
+        <v>45485</v>
       </c>
       <c r="D60" t="s">
         <v>81</v>
       </c>
       <c r="E60">
-        <v>-100.54</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61">
-        <v>291</v>
+        <v>124</v>
       </c>
       <c r="B61" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C61" s="2">
-        <v>45447</v>
+        <v>45485</v>
       </c>
       <c r="D61" t="s">
         <v>82</v>
       </c>
       <c r="E61">
-        <v>-104.94</v>
+        <v>450</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62">
-        <v>594</v>
+        <v>125</v>
       </c>
       <c r="B62" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C62" s="2">
-        <v>45446</v>
+        <v>45485</v>
       </c>
       <c r="D62" t="s">
         <v>83</v>
       </c>
       <c r="E62">
-        <v>-1383.06</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63">
-        <v>703</v>
+        <v>126</v>
       </c>
       <c r="B63" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C63" s="2">
-        <v>45454</v>
+        <v>45483</v>
       </c>
       <c r="D63" t="s">
         <v>84</v>
       </c>
       <c r="E63">
-        <v>1834.75</v>
+        <v>-135000</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64">
-        <v>704</v>
+        <v>127</v>
       </c>
       <c r="B64" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C64" s="2">
-        <v>45446</v>
+        <v>45483</v>
       </c>
       <c r="D64" t="s">
         <v>85</v>
       </c>
       <c r="E64">
-        <v>-843.79</v>
+        <v>-15000</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65">
-        <v>826</v>
+        <v>136</v>
       </c>
       <c r="B65" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C65" s="2">
-        <v>45454</v>
+        <v>45505</v>
       </c>
       <c r="D65" t="s">
         <v>86</v>
       </c>
       <c r="E65">
-        <v>1510</v>
+        <v>-711.48</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66">
-        <v>827</v>
+        <v>137</v>
       </c>
       <c r="B66" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C66" s="2">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="D66" t="s">
         <v>87</v>
       </c>
       <c r="E66">
-        <v>-675.63</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67">
-        <v>904</v>
+        <v>138</v>
       </c>
       <c r="B67" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C67" s="2">
-        <v>45455</v>
+        <v>45504</v>
       </c>
       <c r="D67" t="s">
         <v>88</v>
       </c>
       <c r="E67">
-        <v>-12.07</v>
+        <v>2295</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68">
-        <v>905</v>
+        <v>139</v>
       </c>
       <c r="B68" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C68" s="2">
-        <v>45454</v>
+        <v>45483</v>
       </c>
       <c r="D68" t="s">
         <v>89</v>
       </c>
       <c r="E68">
-        <v>-46.18</v>
+        <v>1823.14</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69">
-        <v>906</v>
+        <v>140</v>
       </c>
       <c r="B69" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C69" s="2">
-        <v>45454</v>
+        <v>45474</v>
       </c>
       <c r="D69" t="s">
         <v>90</v>
       </c>
       <c r="E69">
-        <v>3140.56</v>
+        <v>-711.48</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70">
-        <v>907</v>
+        <v>141</v>
       </c>
       <c r="B70" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C70" s="2">
-        <v>45450</v>
+        <v>45474</v>
       </c>
       <c r="D70" t="s">
         <v>91</v>
       </c>
       <c r="E70">
-        <v>-190.78</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71">
-        <v>908</v>
+        <v>144</v>
       </c>
       <c r="B71" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C71" s="2">
-        <v>45447</v>
+        <v>45506</v>
       </c>
       <c r="D71" t="s">
         <v>92</v>
       </c>
       <c r="E71">
-        <v>-22.15</v>
+        <v>-694.01</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72">
-        <v>909</v>
+        <v>145</v>
       </c>
       <c r="B72" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C72" s="2">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="D72" t="s">
         <v>93</v>
       </c>
       <c r="E72">
+        <v>-75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73">
+        <v>146</v>
+      </c>
+      <c r="B73" t="s">
+        <v>19</v>
+      </c>
+      <c r="C73" s="2">
+        <v>45483</v>
+      </c>
+      <c r="D73" t="s">
+        <v>94</v>
+      </c>
+      <c r="E73">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74">
+        <v>147</v>
+      </c>
+      <c r="B74" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" s="2">
+        <v>45475</v>
+      </c>
+      <c r="D74" t="s">
+        <v>95</v>
+      </c>
+      <c r="E74">
+        <v>-694.01</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75">
+        <v>148</v>
+      </c>
+      <c r="B75" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" s="2">
+        <v>45474</v>
+      </c>
+      <c r="D75" t="s">
+        <v>96</v>
+      </c>
+      <c r="E75">
+        <v>-75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76">
+        <v>152</v>
+      </c>
+      <c r="B76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" s="2">
+        <v>45504</v>
+      </c>
+      <c r="D76" t="s">
+        <v>97</v>
+      </c>
+      <c r="E76">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77">
+        <v>153</v>
+      </c>
+      <c r="B77" t="s">
+        <v>20</v>
+      </c>
+      <c r="C77" s="2">
+        <v>45504</v>
+      </c>
+      <c r="D77" t="s">
+        <v>98</v>
+      </c>
+      <c r="E77">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78">
+        <v>154</v>
+      </c>
+      <c r="B78" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78" s="2">
+        <v>45502</v>
+      </c>
+      <c r="D78" t="s">
+        <v>99</v>
+      </c>
+      <c r="E78">
+        <v>-358.39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79">
+        <v>155</v>
+      </c>
+      <c r="B79" t="s">
+        <v>20</v>
+      </c>
+      <c r="C79" s="2">
+        <v>45474</v>
+      </c>
+      <c r="D79" t="s">
+        <v>100</v>
+      </c>
+      <c r="E79">
+        <v>-96.29000000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80">
+        <v>202</v>
+      </c>
+      <c r="B80" t="s">
+        <v>21</v>
+      </c>
+      <c r="C80" s="2">
+        <v>45504</v>
+      </c>
+      <c r="D80" t="s">
+        <v>101</v>
+      </c>
+      <c r="E80">
+        <v>-248</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81">
+        <v>274</v>
+      </c>
+      <c r="B81" t="s">
+        <v>22</v>
+      </c>
+      <c r="C81" s="2">
+        <v>45504</v>
+      </c>
+      <c r="D81" t="s">
+        <v>102</v>
+      </c>
+      <c r="E81">
+        <v>-1118.25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82">
+        <v>275</v>
+      </c>
+      <c r="B82" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82" s="2">
+        <v>45502</v>
+      </c>
+      <c r="D82" t="s">
+        <v>103</v>
+      </c>
+      <c r="E82">
+        <v>-500</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83">
+        <v>276</v>
+      </c>
+      <c r="B83" t="s">
+        <v>22</v>
+      </c>
+      <c r="C83" s="2">
+        <v>45495</v>
+      </c>
+      <c r="D83" t="s">
+        <v>104</v>
+      </c>
+      <c r="E83">
+        <v>1699.24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84">
+        <v>277</v>
+      </c>
+      <c r="B84" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84" s="2">
+        <v>45483</v>
+      </c>
+      <c r="D84" t="s">
+        <v>105</v>
+      </c>
+      <c r="E84">
+        <v>-46.3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85">
+        <v>278</v>
+      </c>
+      <c r="B85" t="s">
+        <v>22</v>
+      </c>
+      <c r="C85" s="2">
+        <v>45483</v>
+      </c>
+      <c r="D85" t="s">
+        <v>106</v>
+      </c>
+      <c r="E85">
+        <v>-49.54</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86">
+        <v>279</v>
+      </c>
+      <c r="B86" t="s">
+        <v>22</v>
+      </c>
+      <c r="C86" s="2">
+        <v>45483</v>
+      </c>
+      <c r="D86" t="s">
+        <v>107</v>
+      </c>
+      <c r="E86">
+        <v>-70.08</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87">
+        <v>280</v>
+      </c>
+      <c r="B87" t="s">
+        <v>22</v>
+      </c>
+      <c r="C87" s="2">
+        <v>45483</v>
+      </c>
+      <c r="D87" t="s">
+        <v>108</v>
+      </c>
+      <c r="E87">
+        <v>-134.46</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88">
+        <v>281</v>
+      </c>
+      <c r="B88" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" s="2">
+        <v>45483</v>
+      </c>
+      <c r="D88" t="s">
+        <v>109</v>
+      </c>
+      <c r="E88">
+        <v>1504.75</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89">
+        <v>282</v>
+      </c>
+      <c r="B89" t="s">
+        <v>22</v>
+      </c>
+      <c r="C89" s="2">
+        <v>45476</v>
+      </c>
+      <c r="D89" t="s">
+        <v>110</v>
+      </c>
+      <c r="E89">
+        <v>-51.49</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90">
+        <v>283</v>
+      </c>
+      <c r="B90" t="s">
+        <v>22</v>
+      </c>
+      <c r="C90" s="2">
+        <v>45476</v>
+      </c>
+      <c r="D90" t="s">
+        <v>111</v>
+      </c>
+      <c r="E90">
+        <v>-95.72</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91">
+        <v>284</v>
+      </c>
+      <c r="B91" t="s">
+        <v>22</v>
+      </c>
+      <c r="C91" s="2">
+        <v>45476</v>
+      </c>
+      <c r="D91" t="s">
+        <v>112</v>
+      </c>
+      <c r="E91">
+        <v>-143.42</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92">
+        <v>285</v>
+      </c>
+      <c r="B92" t="s">
+        <v>22</v>
+      </c>
+      <c r="C92" s="2">
+        <v>45476</v>
+      </c>
+      <c r="D92" t="s">
+        <v>113</v>
+      </c>
+      <c r="E92">
+        <v>-148.43</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93">
+        <v>592</v>
+      </c>
+      <c r="B93" t="s">
+        <v>23</v>
+      </c>
+      <c r="C93" s="2">
+        <v>45505</v>
+      </c>
+      <c r="D93" t="s">
+        <v>114</v>
+      </c>
+      <c r="E93">
+        <v>-1383.06</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94">
+        <v>593</v>
+      </c>
+      <c r="B94" t="s">
+        <v>23</v>
+      </c>
+      <c r="C94" s="2">
+        <v>45504</v>
+      </c>
+      <c r="D94" t="s">
+        <v>115</v>
+      </c>
+      <c r="E94">
+        <v>6414.53</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95">
+        <v>594</v>
+      </c>
+      <c r="B95" t="s">
+        <v>23</v>
+      </c>
+      <c r="C95" s="2">
+        <v>45474</v>
+      </c>
+      <c r="D95" t="s">
+        <v>116</v>
+      </c>
+      <c r="E95">
+        <v>-1383.06</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96">
+        <v>695</v>
+      </c>
+      <c r="B96" t="s">
+        <v>24</v>
+      </c>
+      <c r="C96" s="2">
+        <v>45505</v>
+      </c>
+      <c r="D96" t="s">
+        <v>117</v>
+      </c>
+      <c r="E96">
+        <v>-843.79</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97">
+        <v>696</v>
+      </c>
+      <c r="B97" t="s">
+        <v>24</v>
+      </c>
+      <c r="C97" s="2">
+        <v>45483</v>
+      </c>
+      <c r="D97" t="s">
+        <v>118</v>
+      </c>
+      <c r="E97">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98">
+        <v>697</v>
+      </c>
+      <c r="B98" t="s">
+        <v>24</v>
+      </c>
+      <c r="C98" s="2">
+        <v>45474</v>
+      </c>
+      <c r="D98" t="s">
+        <v>119</v>
+      </c>
+      <c r="E98">
+        <v>-843.79</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99">
+        <v>814</v>
+      </c>
+      <c r="B99" t="s">
+        <v>25</v>
+      </c>
+      <c r="C99" s="2">
+        <v>45505</v>
+      </c>
+      <c r="D99" t="s">
+        <v>120</v>
+      </c>
+      <c r="E99">
+        <v>-675.63</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100">
+        <v>815</v>
+      </c>
+      <c r="B100" t="s">
+        <v>25</v>
+      </c>
+      <c r="C100" s="2">
+        <v>45483</v>
+      </c>
+      <c r="D100" t="s">
+        <v>121</v>
+      </c>
+      <c r="E100">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101">
+        <v>816</v>
+      </c>
+      <c r="B101" t="s">
+        <v>25</v>
+      </c>
+      <c r="C101" s="2">
+        <v>45474</v>
+      </c>
+      <c r="D101" t="s">
+        <v>122</v>
+      </c>
+      <c r="E101">
+        <v>-675.63</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102">
+        <v>889</v>
+      </c>
+      <c r="B102" t="s">
+        <v>26</v>
+      </c>
+      <c r="C102" s="2">
+        <v>45505</v>
+      </c>
+      <c r="D102" t="s">
+        <v>123</v>
+      </c>
+      <c r="E102">
+        <v>-1383.06</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103">
+        <v>890</v>
+      </c>
+      <c r="B103" t="s">
+        <v>26</v>
+      </c>
+      <c r="C103" s="2">
+        <v>45483</v>
+      </c>
+      <c r="D103" t="s">
+        <v>124</v>
+      </c>
+      <c r="E103">
+        <v>2655</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104">
+        <v>891</v>
+      </c>
+      <c r="B104" t="s">
+        <v>26</v>
+      </c>
+      <c r="C104" s="2">
+        <v>45474</v>
+      </c>
+      <c r="D104" t="s">
+        <v>125</v>
+      </c>
+      <c r="E104">
         <v>-1383.06</v>
       </c>
     </row>

</xml_diff>